<commit_message>
actualizado el diagrama burndown
</commit_message>
<xml_diff>
--- a/documentos/SPRINTS/SPRINT1/archivos/DIAGRAMA BURNDOWN SGAL.xlsx
+++ b/documentos/SPRINTS/SPRINT1/archivos/DIAGRAMA BURNDOWN SGAL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\egobr\Dropbox\21-Direccion_Gestion_Proyectos\1_Gestion_Alumnos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3F765F36-B888-4714-BB12-10F465703FD8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C84F03DB-5CC0-4063-B2D4-340395F857D2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="262" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -297,7 +297,235 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
+  <dxfs count="38">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -593,13 +821,13 @@
                   <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>7</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>7</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>7</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2153,8 +2381,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:Q37"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="O5" sqref="O5"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A17" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J37" sqref="J37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -2309,12 +2537,14 @@
       <c r="J31" s="6">
         <v>1</v>
       </c>
-      <c r="K31" s="6"/>
+      <c r="K31" s="6">
+        <v>1</v>
+      </c>
       <c r="L31" s="6"/>
       <c r="M31" s="6"/>
       <c r="N31" s="6">
         <f t="shared" ref="N31:N33" si="0">SUM(D31:M31)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="O31" s="5"/>
       <c r="Q31" s="5"/>
@@ -2371,12 +2601,14 @@
       <c r="J33" s="6">
         <v>2</v>
       </c>
-      <c r="K33" s="6"/>
+      <c r="K33" s="6">
+        <v>1</v>
+      </c>
       <c r="L33" s="6"/>
       <c r="M33" s="6"/>
       <c r="N33" s="6">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="O33" s="5"/>
       <c r="Q33" s="5"/>
@@ -2438,19 +2670,19 @@
       </c>
       <c r="K35" s="18">
         <f t="shared" si="1"/>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="L35" s="18">
         <f t="shared" si="1"/>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="M35" s="18">
         <f t="shared" si="1"/>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="N35" s="19">
         <f xml:space="preserve"> SUM(N29:N33)</f>
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="O35" s="5"/>
       <c r="Q35" s="5"/>
@@ -2541,7 +2773,7 @@
       </c>
       <c r="K37" s="15" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>OK</v>
       </c>
       <c r="L37" s="15" t="str">
         <f t="shared" si="3"/>
@@ -2555,7 +2787,7 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="D37:N37">
-    <cfRule type="iconSet" priority="23">
+    <cfRule type="iconSet" priority="32">
       <iconSet iconSet="3Flags">
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="33"/>
@@ -2564,61 +2796,108 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N35">
-    <cfRule type="cellIs" dxfId="11" priority="17" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="37" priority="26" operator="greaterThanOrEqual">
       <formula>$N$36</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J35">
-    <cfRule type="cellIs" dxfId="10" priority="13" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="36" priority="22" operator="lessThanOrEqual">
       <formula>$J$36</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E35">
-    <cfRule type="cellIs" dxfId="9" priority="11" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="35" priority="20" operator="lessThanOrEqual">
       <formula>$E$36</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="8" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="34" priority="17" operator="lessThanOrEqual">
       <formula>$E$36</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D35">
-    <cfRule type="cellIs" dxfId="7" priority="9" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="33" priority="18" operator="lessThanOrEqual">
       <formula>$D$36</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F35">
-    <cfRule type="cellIs" dxfId="6" priority="7" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="32" priority="16" operator="lessThanOrEqual">
       <formula>$F$36</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G35">
-    <cfRule type="cellIs" dxfId="5" priority="6" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="31" priority="15" operator="lessThanOrEqual">
       <formula>$G$36</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H35">
-    <cfRule type="cellIs" dxfId="4" priority="5" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="30" priority="14" operator="lessThanOrEqual">
       <formula>$H$36</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I35">
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="29" priority="13" operator="lessThanOrEqual">
       <formula>$I$36</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K35">
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="28" priority="12" operator="lessThanOrEqual">
       <formula>$K$36</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L35">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="27" priority="11" operator="lessThanOrEqual">
       <formula>$L$36</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M35">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="26" priority="10" operator="lessThanOrEqual">
       <formula>$M$36</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N29">
+    <cfRule type="cellIs" dxfId="25" priority="9" operator="equal">
+      <formula>$C$29</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="24" priority="7" operator="equal">
+      <formula>$C$29</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N30">
+    <cfRule type="cellIs" dxfId="23" priority="8" operator="equal">
+      <formula>$C$30</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N31">
+    <cfRule type="cellIs" dxfId="22" priority="6" operator="equal">
+      <formula>$C$31</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N32">
+    <cfRule type="cellIs" dxfId="21" priority="5" operator="equal">
+      <formula>"$C$32"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="20" priority="3" operator="equal">
+      <formula>$C$32</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N33">
+    <cfRule type="cellIs" dxfId="19" priority="4" operator="equal">
+      <formula>$C$33</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J37">
+    <cfRule type="iconSet" priority="2">
+      <iconSet iconSet="3Flags">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="percent" val="33"/>
+        <cfvo type="percent" val="67"/>
+      </iconSet>
+    </cfRule>
+    <cfRule type="iconSet" priority="1">
+      <iconSet>
+        <cfvo type="percent" val="0"/>
+        <cfvo type="percent" val="33"/>
+        <cfvo type="num" val="&quot;si+$J$35&lt;$J$36&quot;"/>
+      </iconSet>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>